<commit_message>
fixed errorsin excel sheet
</commit_message>
<xml_diff>
--- a/Convex_hull_plot.xlsx
+++ b/Convex_hull_plot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE projects\Convex Hull Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE projects\Convex Hull Project\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B0611-0590-484C-8D97-B18018F69E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89D01CE-EA0B-4ECB-A9D6-9E5A87466F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3192" yWindow="2976" windowWidth="10380" windowHeight="9420" xr2:uid="{0F8E8E9B-D5D1-45A8-931C-065DF12F457C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0F8E8E9B-D5D1-45A8-931C-065DF12F457C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>X - Coordinate</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -53,7 +50,10 @@
     <t>X- Coordinate</t>
   </si>
   <si>
-    <t>Y - Coordiante</t>
+    <t>X - Coordiante</t>
+  </si>
+  <si>
+    <t>Y - Coordinate</t>
   </si>
 </sst>
 </file>
@@ -178,10 +178,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.1281245601397623E-2"/>
-          <c:y val="4.8765396555777871E-2"/>
-          <c:w val="0.86807359845003607"/>
-          <c:h val="0.77353111939618147"/>
+          <c:x val="8.0862985968396181E-2"/>
+          <c:y val="3.2107413893753649E-2"/>
+          <c:w val="0.85393566090162465"/>
+          <c:h val="0.7857922127203979"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -191,13 +191,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Convex Hull Points</c:v>
+            <c:v>Input Points</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -219,84 +217,618 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>929</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>956</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>932</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>865</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>497</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>921</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>987</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>858</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="98">
                   <c:v>143</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>739</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>932</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>987</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>859</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>143</c:v>
+                <c:pt idx="99">
+                  <c:v>928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:f>Sheet1!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>926</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>873</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>857</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>895</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>808</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>902</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>927</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>965</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>683</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>871</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>829</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="98">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>856</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>936</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>965</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>980</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>764</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
+                <c:pt idx="99">
+                  <c:v>529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -304,7 +836,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A89C-40CE-9CEA-E995F56F774C}"/>
+              <c16:uniqueId val="{00000000-F531-42D1-AFDE-DFB370841797}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -312,11 +844,13 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Input Points</c:v>
+            <c:v>Convex Hall Points</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -338,618 +872,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$101</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>886</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>915</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>335</c:v>
+                  <c:v>932</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>492</c:v>
+                  <c:v>996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>421</c:v>
+                  <c:v>987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>859</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>926</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>426</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>736</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>429</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>530</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>802</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>456</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>373</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>919</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>537</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>526</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>980</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>873</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>925</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>327</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>505</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>857</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>895</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>545</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>367</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>808</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>584</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>651</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>399</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>539</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>570</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>378</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>601</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>902</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>492</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>756</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>441</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>689</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>619</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>771</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>927</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>856</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>353</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>965</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>683</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>624</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>871</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>829</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>715</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>149</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>723</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>451</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>555</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>488</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>764</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>914</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>856</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>491</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>936</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>551</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>407</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>793</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>428</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>529</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>383</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>777</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>793</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>386</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>649</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>362</c:v>
+                  <c:v>936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>690</c:v>
+                  <c:v>965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>763</c:v>
+                  <c:v>980</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>540</c:v>
+                  <c:v>764</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>172</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>567</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>782</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>862</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>929</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>393</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>784</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>413</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>956</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>862</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>996</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>846</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>313</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>582</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>814</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>434</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>788</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>754</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>932</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>676</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>739</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>795</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>434</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>467</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>652</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>286</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>865</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>444</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>481</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>709</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>567</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>497</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>528</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>732</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>503</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>708</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>796</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>618</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>846</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>921</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>764</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>841</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>987</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>743</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>859</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>437</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>474</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>858</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>818</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,7 +957,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A89C-40CE-9CEA-E995F56F774C}"/>
+              <c16:uniqueId val="{00000001-F531-42D1-AFDE-DFB370841797}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -969,11 +969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117884255"/>
-        <c:axId val="117145503"/>
+        <c:axId val="2063219839"/>
+        <c:axId val="2062125439"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="117884255"/>
+        <c:axId val="2063219839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,12 +1030,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117145503"/>
+        <c:crossAx val="2062125439"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117145503"/>
+        <c:axId val="2062125439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117884255"/>
+        <c:crossAx val="2063219839"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1105,7 +1105,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3143685393431393"/>
+          <c:y val="0.87923685744101265"/>
+          <c:w val="0.2471134592218526"/>
+          <c:h val="9.8339849127250717E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1739,23 +1749,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1425D533-C23B-4F29-8961-3A9640045E5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A66CD34-2B1D-4EF5-A760-863F970B67F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2075,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A605A21D-8640-4D70-A7B5-DBC5EA71EA33}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,16 +2102,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2311,7 +2321,6 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -2322,7 +2331,6 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -2333,7 +2341,6 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -2344,7 +2351,6 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -2355,7 +2361,6 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -2366,7 +2371,6 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -2377,7 +2381,6 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -2388,7 +2391,6 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -2399,7 +2401,6 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
@@ -2410,7 +2411,6 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -2421,7 +2421,6 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -2432,7 +2431,6 @@
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -2443,7 +2441,6 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">

</xml_diff>